<commit_message>
Ajout remplisage gazon à coté des tents
</commit_message>
<xml_diff>
--- a/SousImageCMieux.xlsx
+++ b/SousImageCMieux.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louischaumont\Desktop\PROJET_DES_TENTES_ET_DES_ARBRES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louischaumont\Desktop\DesTentesEtDesArbres-Solver\DesTentesEtDesAbres-Solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0329679F-3107-4874-AB90-F79198CAFC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4830A885-499D-4787-B8D2-FE8AADA360B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BFC321B-3400-4F7A-BC7A-5CCDF2EBFB2F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
   <si>
     <t>---------------</t>
   </si>
@@ -109,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -133,6 +133,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C4B87D-80F3-4545-AB54-32521CE7EA12}">
   <dimension ref="A1:XFD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,9 +578,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
+      <c r="L5" s="2"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="5"/>
@@ -598,9 +599,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2">
-        <v>3</v>
-      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="6"/>
@@ -621,9 +620,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="6"/>
       <c r="N7" s="5"/>
       <c r="O7" s="3"/>
@@ -672,37 +669,17 @@
       <c r="J9" s="2"/>
       <c r="K9" s="7"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2">
-        <v>2</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <v>2</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>2</v>
-      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="T9" s="2">
-        <v>2</v>
-      </c>
-      <c r="U9" s="2">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2">
-        <v>2</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
-        <v>2</v>
-      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
     </row>
     <row r="10" spans="1:24" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -718,17 +695,13 @@
       <c r="I10" s="4"/>
       <c r="J10" s="2"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
+      <c r="L10" s="2"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="6"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="3"/>
-      <c r="S10" s="2">
-        <v>1</v>
-      </c>
+      <c r="S10" s="2"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -749,17 +722,13 @@
       <c r="I11" s="4"/>
       <c r="J11" s="2"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="2">
-        <v>2</v>
-      </c>
+      <c r="L11" s="2"/>
       <c r="M11" s="6"/>
       <c r="N11" s="5"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="6"/>
-      <c r="S11" s="2">
-        <v>2</v>
-      </c>
+      <c r="S11" s="2"/>
       <c r="T11" s="6"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
@@ -780,17 +749,13 @@
       <c r="I12" s="5"/>
       <c r="J12" s="2"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
+      <c r="L12" s="2"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="5"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="5"/>
-      <c r="S12" s="2">
-        <v>0</v>
-      </c>
+      <c r="S12" s="2"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="5"/>
@@ -811,17 +776,13 @@
       <c r="I13" s="4"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <v>2</v>
-      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="6"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="6"/>
-      <c r="S13" s="2">
-        <v>2</v>
-      </c>
+      <c r="S13" s="2"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="6"/>
@@ -842,17 +803,13 @@
       <c r="I14" s="3"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
+      <c r="L14" s="2"/>
       <c r="M14" s="6"/>
       <c r="N14" s="5"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="S14" s="2">
-        <v>1</v>
-      </c>
+      <c r="S14" s="2"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="3"/>
@@ -919,12 +876,8 @@
       <c r="I17" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -978,44 +931,20 @@
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2">
-        <v>3</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2">
-        <v>1</v>
-      </c>
-      <c r="O19" s="2">
-        <v>1</v>
-      </c>
-      <c r="P19" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
-      <c r="T19" s="2">
-        <v>3</v>
-      </c>
-      <c r="U19" s="2">
-        <v>0</v>
-      </c>
-      <c r="V19" s="2">
-        <v>1</v>
-      </c>
-      <c r="W19" s="2">
-        <v>1</v>
-      </c>
-      <c r="X19" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="2">
-        <v>1</v>
-      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
     </row>
     <row r="20" spans="1:25 16384:16384" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1030,9 +959,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="2">
-        <v>1</v>
-      </c>
+      <c r="K20" s="2"/>
       <c r="L20" s="6"/>
       <c r="M20" s="3"/>
       <c r="N20" s="5"/>
@@ -1040,9 +967,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="2">
-        <v>1</v>
-      </c>
+      <c r="S20" s="2"/>
       <c r="T20" s="6"/>
       <c r="U20" s="3"/>
       <c r="V20" s="5"/>
@@ -1060,9 +985,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
       <c r="I21" s="4"/>
-      <c r="K21" s="2">
-        <v>2</v>
-      </c>
+      <c r="K21" s="2"/>
       <c r="L21" s="5"/>
       <c r="M21" s="3"/>
       <c r="N21" s="6"/>
@@ -1070,9 +993,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="2">
-        <v>2</v>
-      </c>
+      <c r="S21" s="2"/>
       <c r="T21" s="5"/>
       <c r="U21" s="3"/>
       <c r="V21" s="6"/>
@@ -1090,9 +1011,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
+      <c r="K22" s="2"/>
       <c r="L22" s="6"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1100,9 +1019,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="2">
-        <v>1</v>
-      </c>
+      <c r="S22" s="2"/>
       <c r="T22" s="6"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -1120,9 +1037,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="K23" s="2">
-        <v>1</v>
-      </c>
+      <c r="K23" s="2"/>
       <c r="L23" s="5"/>
       <c r="M23" s="3"/>
       <c r="N23" s="4"/>
@@ -1130,9 +1045,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2">
-        <v>1</v>
-      </c>
+      <c r="S23" s="2"/>
       <c r="T23" s="5"/>
       <c r="U23" s="3"/>
       <c r="V23" s="4"/>
@@ -1150,9 +1063,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
-      <c r="K24" s="2">
-        <v>2</v>
-      </c>
+      <c r="K24" s="2"/>
       <c r="L24" s="6"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
@@ -1160,9 +1071,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2">
-        <v>2</v>
-      </c>
+      <c r="S24" s="2"/>
       <c r="T24" s="6"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
@@ -1180,18 +1089,14 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
-      <c r="K25" s="2">
-        <v>1</v>
-      </c>
+      <c r="K25" s="2"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="4"/>
       <c r="O25" s="3"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="5"/>
-      <c r="S25" s="2">
-        <v>1</v>
-      </c>
+      <c r="S25" s="2"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="4"/>
@@ -1200,28 +1105,427 @@
       <c r="Y25" s="5"/>
     </row>
     <row r="26" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2">
+        <v>3</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
+      <c r="R27" s="2">
+        <v>2</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="2">
+        <v>2</v>
+      </c>
+      <c r="M28" s="6"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="2">
+        <v>2</v>
+      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="2">
+        <v>2</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="1:25 16384:16384" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" s="6"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="2">
+        <v>1</v>
+      </c>
+      <c r="M33" s="4"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="4"/>
+    </row>
+    <row r="34" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="L34" s="2">
+        <v>2</v>
+      </c>
+      <c r="M34" s="4"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2">
+        <v>3</v>
+      </c>
+      <c r="N36" s="2">
+        <v>1</v>
+      </c>
+      <c r="O36" s="2">
+        <v>1</v>
+      </c>
+      <c r="P36" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>1</v>
+      </c>
+      <c r="R36" s="2">
+        <v>2</v>
+      </c>
+      <c r="S36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="4"/>
+      <c r="L37" s="2">
+        <v>2</v>
+      </c>
+      <c r="M37" s="6"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="6"/>
+    </row>
+    <row r="38" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="3"/>
+      <c r="L38" s="2">
+        <v>2</v>
+      </c>
+      <c r="M38" s="5"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="L39" s="2">
+        <v>1</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="3"/>
+      <c r="L40" s="2">
+        <v>2</v>
+      </c>
+      <c r="M40" s="5"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+      <c r="M41" s="6"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+    </row>
+    <row r="42" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="3"/>
+      <c r="L42" s="2">
+        <v>1</v>
+      </c>
+      <c r="M42" s="4"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="L43" s="2">
+        <v>2</v>
+      </c>
+      <c r="M43" s="3"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+    </row>
+    <row r="44" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>